<commit_message>
altera data por excel
</commit_message>
<xml_diff>
--- a/usuario.xlsx
+++ b/usuario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03e5503c98df8318/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22AE1869-244B-4A46-8CE7-A2719CBD8DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{22AE1869-244B-4A46-8CE7-A2719CBD8DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA8C1FD7-23EC-43FC-8E83-EFA15DF6FB4E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F6486409-E64A-4DF3-9F6F-EA3008F7FB69}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>usuario</t>
-  </si>
-  <si>
     <t>usuarios</t>
   </si>
   <si>
@@ -54,14 +51,25 @@
   </si>
   <si>
     <t>usuario 3</t>
+  </si>
+  <si>
+    <t>nome</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -89,11 +97,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,28 +440,28 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B3">
         <v>30</v>
@@ -460,7 +469,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -468,7 +477,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>20</v>

</xml_diff>